<commit_message>
Dodanie klasy ModifyDatabase, mozliwosc modyfikacji kordow wybranego wektora
</commit_message>
<xml_diff>
--- a/database/UserDatabase.xlsx
+++ b/database/UserDatabase.xlsx
@@ -55,7 +55,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -89,6 +89,20 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>-4.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>